<commit_message>
Solved part 3. Completed reports for part 2 and 3. Cleanup.
</commit_message>
<xml_diff>
--- a/performance_benchmarking.xlsx
+++ b/performance_benchmarking.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Selectors" sheetId="1" r:id="rId1"/>
+    <sheet name="WER" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="37">
   <si>
     <t>CV</t>
   </si>
@@ -114,6 +115,30 @@
   </si>
   <si>
     <t>Avf Feature Perf</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Model Selector</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>WER</t>
+  </si>
+  <si>
+    <t>Correct words</t>
+  </si>
+  <si>
+    <t>Constant 3</t>
+  </si>
+  <si>
+    <t>Constant 4</t>
+  </si>
+  <si>
+    <t>Constant 7</t>
   </si>
 </sst>
 </file>
@@ -137,7 +162,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,8 +181,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -300,14 +343,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -318,9 +435,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -598,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M85"/>
+  <dimension ref="B1:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86:F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,1408 +749,2038 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>5</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>129</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <f>AVERAGE(F3:F7)</f>
         <v>-1743.4</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="13">
         <f>MIN(E3,E8,E13,E18)</f>
         <v>4</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="1">
         <f>MAX(E3,E8,E13,E18)</f>
         <v>8</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="1">
         <f>AVERAGE(E3,E8,E13,E18)</f>
         <v>6</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="1">
         <f>MIN(F3,F8,F13,F18)</f>
         <v>129</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="1">
         <f>MAX(F3,F8,F13,F18)</f>
         <v>216</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="6">
         <f>AVERAGE(F3,F8,F13,F18)</f>
         <v>171.25</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>6</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>-872</v>
       </c>
-      <c r="H4" s="7">
+      <c r="G4" s="6"/>
+      <c r="H4" s="13">
         <f>MIN(E4,E9,E14,E19)</f>
         <v>5</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="1">
         <f>MAX(E4,E9,E14,E19)</f>
         <v>9</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="1">
         <f>AVERAGE(E4,E9,E14,E19)</f>
         <v>7</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="1">
         <f>MIN(F4,F9,F14,F19)</f>
         <v>-872</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="1">
         <f>MAX(F4,F9,F14,F19)</f>
         <v>199</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="6">
         <f>AVERAGE(F4,F9,F14,F19)</f>
         <v>-324.75</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>-733</v>
       </c>
-      <c r="H5" s="7">
+      <c r="G5" s="6"/>
+      <c r="H5" s="13">
         <f>MIN(E5,E10,E15,E20)</f>
         <v>2</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="1">
         <f>MAX(E5,E10,E15,E20)</f>
         <v>15</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="1">
         <f>AVERAGE(E5,E10,E15,E20)</f>
         <v>6</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="1">
         <f>MIN(F5,F10,F15,F20)</f>
         <v>-733</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="1">
         <f>MAX(F5,F10,F15,F20)</f>
         <v>180</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="6">
         <f>AVERAGE(F5,F10,F15,F20)</f>
         <v>-227.25</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>-823</v>
       </c>
-      <c r="H6" s="7">
+      <c r="G6" s="6"/>
+      <c r="H6" s="13">
         <f>MIN(E6,E11,E16,E21)</f>
         <v>2</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="1">
         <f>MAX(E6,E11,E16,E21)</f>
         <v>3</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="1">
         <f>AVERAGE(E6,E11,E16,E21)</f>
         <v>2.25</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="1">
         <f>MIN(F6,F11,F16,F21)</f>
         <v>-823</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="1">
         <f>MAX(F6,F11,F16,F21)</f>
         <v>160</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="6">
         <f>AVERAGE(F6,F11,F16,F21)</f>
         <v>-313.75</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="8">
         <v>12</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="8">
         <v>-6418</v>
       </c>
-      <c r="H7" s="9">
+      <c r="G7" s="9"/>
+      <c r="H7" s="14">
         <f>MIN(E7,E12,E17,E22)</f>
         <v>8</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="8">
         <f>MAX(E7,E12,E17,E22)</f>
         <v>14</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="8">
         <f>AVERAGE(E7,E12,E17,E22)</f>
         <v>10.75</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="8">
         <f>MIN(F7,F12,F17,F22)</f>
         <v>-6418</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="8">
         <f>MAX(F7,F12,F17,F22)</f>
         <v>3140</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="9">
         <f>AVERAGE(F7,F12,F17,F22)</f>
         <v>-1485.5</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>8</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>177</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="4">
         <f>AVERAGE(F8:F12)</f>
         <v>-764.8</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>5</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>-388</v>
       </c>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D10" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E10">
-        <v>15</v>
-      </c>
-      <c r="F10">
+      <c r="E10" s="1">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1">
         <v>-506</v>
       </c>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D11" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>2</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>-400</v>
       </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D12" t="s">
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="8">
         <v>14</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="8">
         <v>-2707</v>
       </c>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>4</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>163</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="4">
         <f>AVERAGE(F13:F17)</f>
         <v>-14.8</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D14" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>9</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>-238</v>
       </c>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D15" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>5</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>150</v>
       </c>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D16" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>2</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>-192</v>
       </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D17" t="s">
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="8">
         <v>8</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="8">
         <v>43</v>
       </c>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <v>7</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>216</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="4">
         <f>AVERAGE(F18:F22)</f>
         <v>779</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D19" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>8</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>199</v>
       </c>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D20" t="s">
+      <c r="B20" s="1"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>2</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>180</v>
       </c>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D21" t="s">
+      <c r="B21" s="1"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>3</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>160</v>
       </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D22" t="s">
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="8">
         <v>9</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="8">
         <v>3140</v>
       </c>
+      <c r="G22" s="9"/>
     </row>
     <row r="24" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
+    <row r="25" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C25" s="1"/>
+      <c r="D25" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="G25" s="17"/>
+      <c r="H25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="I25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="K25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="L25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M25" s="6" t="s">
+      <c r="M25" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="3">
         <v>5</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>-228</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="4">
         <f>AVERAGE(F26:F30)</f>
         <v>9840.7999999999993</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="13">
         <f>MIN(E26,E31,E36,E41)</f>
         <v>4</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="1">
         <f>MAX(E26,E31,E36,E41)</f>
         <v>6</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="1">
         <f>AVERAGE(E26,E31,E36,E41)</f>
         <v>4.75</v>
       </c>
-      <c r="K26" s="3">
+      <c r="K26" s="1">
         <f>MIN(F26,F31,F36,F41)</f>
         <v>-410</v>
       </c>
-      <c r="L26" s="3">
+      <c r="L26" s="1">
         <f>MAX(F26,F31,F36,F41)</f>
         <v>-228</v>
       </c>
-      <c r="M26" s="8">
+      <c r="M26" s="6">
         <f>AVERAGE(F26,F31,F36,F41)</f>
         <v>-314.25</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D27" t="s">
+      <c r="B27" s="1"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <v>8</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <v>4776</v>
       </c>
-      <c r="H27" s="7">
+      <c r="G27" s="6"/>
+      <c r="H27" s="13">
         <f>MIN(E27,E32,E37,E42)</f>
         <v>2</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="1">
         <f>MAX(E27,E32,E37,E42)</f>
         <v>8</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="1">
         <f>AVERAGE(E27,E32,E37,E42)</f>
         <v>4.5</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K27" s="1">
         <f>MIN(F27,F32,F37,F42)</f>
         <v>-1182</v>
       </c>
-      <c r="L27" s="3">
+      <c r="L27" s="1">
         <f>MAX(F27,F32,F37,F42)</f>
         <v>4776</v>
       </c>
-      <c r="M27" s="8">
+      <c r="M27" s="6">
         <f>AVERAGE(F27,F32,F37,F42)</f>
         <v>1824</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D28" t="s">
+      <c r="B28" s="1"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>14</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>893</v>
       </c>
-      <c r="H28" s="7">
+      <c r="G28" s="6"/>
+      <c r="H28" s="13">
         <f>MIN(E28,E33,E38,E43)</f>
         <v>2</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="1">
         <f>MAX(E28,E33,E38,E43)</f>
         <v>14</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="1">
         <f>AVERAGE(E28,E33,E38,E43)</f>
         <v>7.25</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K28" s="1">
         <f>MIN(F28,F33,F38,F43)</f>
         <v>-1216</v>
       </c>
-      <c r="L28" s="3">
+      <c r="L28" s="1">
         <f>MAX(F28,F33,F38,F43)</f>
         <v>893</v>
       </c>
-      <c r="M28" s="8">
+      <c r="M28" s="6">
         <f>AVERAGE(F28,F33,F38,F43)</f>
         <v>-367.75</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D29" t="s">
+      <c r="B29" s="1"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <v>4</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <v>4083</v>
       </c>
-      <c r="H29" s="7">
+      <c r="G29" s="6"/>
+      <c r="H29" s="13">
         <f>MIN(E29,E34,E39,E44)</f>
         <v>2</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="1">
         <f>MAX(E29,E34,E39,E44)</f>
         <v>5</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="1">
         <f>AVERAGE(E29,E34,E39,E44)</f>
         <v>3.75</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K29" s="1">
         <f>MIN(F29,F34,F39,F44)</f>
         <v>-1013</v>
       </c>
-      <c r="L29" s="3">
+      <c r="L29" s="1">
         <f>MAX(F29,F34,F39,F44)</f>
         <v>4083</v>
       </c>
-      <c r="M29" s="8">
+      <c r="M29" s="6">
         <f>AVERAGE(F29,F34,F39,F44)</f>
         <v>1365</v>
       </c>
     </row>
     <row r="30" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
+      <c r="B30" s="1"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="8">
         <v>2</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="8">
         <v>39680</v>
       </c>
-      <c r="H30" s="9">
+      <c r="G30" s="9"/>
+      <c r="H30" s="14">
         <f>MIN(E30,E35,E40,E45)</f>
         <v>2</v>
       </c>
-      <c r="I30" s="10">
+      <c r="I30" s="8">
         <f>MAX(E30,E35,E40,E45)</f>
         <v>6</v>
       </c>
-      <c r="J30" s="10">
+      <c r="J30" s="8">
         <f>AVERAGE(E30,E35,E40,E45)</f>
         <v>3.25</v>
       </c>
-      <c r="K30" s="10">
+      <c r="K30" s="8">
         <f>MIN(F30,F35,F40,F45)</f>
         <v>-15849</v>
       </c>
-      <c r="L30" s="10">
+      <c r="L30" s="8">
         <f>MAX(F30,F35,F40,F45)</f>
         <v>39680</v>
       </c>
-      <c r="M30" s="11">
+      <c r="M30" s="9">
         <f>AVERAGE(F30,F35,F40,F45)</f>
         <v>10191</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
+      <c r="B31" s="1"/>
+      <c r="C31" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="3">
         <v>6</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="3">
         <v>-313</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="4">
         <f>AVERAGE(F31:F35)</f>
         <v>4409.3999999999996</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D32" t="s">
+      <c r="B32" s="1"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>5</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <v>2040</v>
       </c>
+      <c r="G32" s="6"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D33" t="s">
+      <c r="B33" s="1"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <v>10</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>56</v>
       </c>
+      <c r="G33" s="6"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D34" t="s">
+      <c r="B34" s="1"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <v>4</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>1748</v>
       </c>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D35" t="s">
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="8">
         <v>3</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="8">
         <v>18516</v>
       </c>
+      <c r="G35" s="9"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
+      <c r="B36" s="1"/>
+      <c r="C36" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="3">
         <v>4</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="3">
         <v>-306</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="4">
         <f>AVERAGE(F36:F40)</f>
         <v>-160.19999999999999</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D37" t="s">
+      <c r="B37" s="1"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <v>3</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="1">
         <v>1662</v>
       </c>
+      <c r="G37" s="6"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D38" t="s">
+      <c r="B38" s="1"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <v>3</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="1">
         <v>-1216</v>
       </c>
+      <c r="G38" s="6"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D39" t="s">
+      <c r="B39" s="1"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="1">
         <v>5</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="1">
         <v>642</v>
       </c>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D40" t="s">
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="8">
         <v>6</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="8">
         <v>-1583</v>
       </c>
+      <c r="G40" s="9"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C41" t="s">
+      <c r="B41" s="1"/>
+      <c r="C41" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="3">
         <v>4</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="3">
         <v>-410</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="4">
         <f>AVERAGE(F41:F45)</f>
         <v>-3931.6</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D42" t="s">
+      <c r="B42" s="1"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="1">
         <v>2</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="1">
         <v>-1182</v>
       </c>
+      <c r="G42" s="6"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D43" t="s">
+      <c r="B43" s="1"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="1">
         <v>2</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="1">
         <v>-1204</v>
       </c>
+      <c r="G43" s="6"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D44" t="s">
+      <c r="B44" s="1"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="1">
         <v>2</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="1">
         <v>-1013</v>
       </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D45" t="s">
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="8">
         <v>2</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="8">
         <v>-15849</v>
       </c>
+      <c r="G45" s="9"/>
     </row>
     <row r="46" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
+    <row r="47" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D47" t="s">
+      <c r="C47" s="1"/>
+      <c r="D47" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="G47" s="17"/>
+      <c r="H47" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I47" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J47" s="5" t="s">
+      <c r="I47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K47" s="5" t="s">
+      <c r="K47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L47" s="5" t="s">
+      <c r="L47" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M47" s="6" t="s">
+      <c r="M47" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="3">
         <v>3</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="3">
         <v>3665494</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="4">
         <f>AVERAGE(F48:F52)</f>
         <v>732798.6</v>
       </c>
-      <c r="H48" s="7">
+      <c r="H48" s="13">
         <f>MIN(E48,E53,E58,E63)</f>
         <v>2</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I48" s="1">
         <f>MAX(E48,E53,E58,E63)</f>
         <v>4</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="1">
         <f>AVERAGE(E48,E53,E58,E63)</f>
         <v>3.25</v>
       </c>
-      <c r="K48" s="3">
+      <c r="K48" s="1">
         <f>MIN(F48,F53,F58,F63)</f>
         <v>507</v>
       </c>
-      <c r="L48" s="3">
+      <c r="L48" s="1">
         <f>MAX(F48,F53,F58,F63)</f>
         <v>3665494</v>
       </c>
-      <c r="M48" s="8">
+      <c r="M48" s="6">
         <f>AVERAGE(F48,F53,F58,F63)</f>
         <v>1503471</v>
       </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D49" t="s">
+      <c r="C49" s="16"/>
+      <c r="D49" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E49">
-        <v>15</v>
-      </c>
-      <c r="F49">
+      <c r="E49" s="1">
+        <v>15</v>
+      </c>
+      <c r="F49" s="1">
         <v>-433</v>
       </c>
-      <c r="H49" s="7">
+      <c r="G49" s="6"/>
+      <c r="H49" s="13">
         <f>MIN(E49,E54,E59,E64)</f>
         <v>13</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49" s="1">
         <f>MAX(E49,E54,E59,E64)</f>
         <v>15</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="1">
         <f>AVERAGE(E49,E54,E59,E64)</f>
         <v>14</v>
       </c>
-      <c r="K49" s="3">
+      <c r="K49" s="1">
         <f>MIN(F49,F54,F59,F64)</f>
         <v>-433</v>
       </c>
-      <c r="L49" s="3">
+      <c r="L49" s="1">
         <f>MAX(F49,F54,F59,F64)</f>
         <v>1384</v>
       </c>
-      <c r="M49" s="8">
+      <c r="M49" s="6">
         <f>AVERAGE(F49,F54,F59,F64)</f>
         <v>463.25</v>
       </c>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D50" t="s">
+      <c r="B50" s="1"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E50">
-        <v>15</v>
-      </c>
-      <c r="F50">
+      <c r="E50" s="1">
+        <v>15</v>
+      </c>
+      <c r="F50" s="1">
         <v>14039</v>
       </c>
-      <c r="H50" s="13">
+      <c r="G50" s="6"/>
+      <c r="H50" s="18">
         <f>MIN(E50,E55,E60,E65)</f>
         <v>2</v>
       </c>
-      <c r="I50" s="12">
+      <c r="I50" s="10">
         <f>MAX(E50,E55,E60,E65)</f>
         <v>15</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="1">
         <f>AVERAGE(E50,E55,E60,E65)</f>
         <v>8.5</v>
       </c>
-      <c r="K50" s="3">
+      <c r="K50" s="1">
         <f>MIN(F50,F55,F60,F65)</f>
         <v>842</v>
       </c>
-      <c r="L50" s="3">
+      <c r="L50" s="1">
         <f>MAX(F50,F55,F60,F65)</f>
         <v>459033</v>
       </c>
-      <c r="M50" s="8">
+      <c r="M50" s="6">
         <f>AVERAGE(F50,F55,F60,F65)</f>
         <v>120968</v>
       </c>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D51" t="s">
+      <c r="B51" s="1"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E51">
-        <v>15</v>
-      </c>
-      <c r="F51">
+      <c r="E51" s="1">
+        <v>15</v>
+      </c>
+      <c r="F51" s="1">
         <v>-148</v>
       </c>
-      <c r="H51" s="7">
+      <c r="G51" s="6"/>
+      <c r="H51" s="13">
         <f>MIN(E51,E56,E61,E66)</f>
         <v>5</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51" s="1">
         <f>MAX(E51,E56,E61,E66)</f>
         <v>15</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="1">
         <f>AVERAGE(E51,E56,E61,E66)</f>
         <v>12.25</v>
       </c>
-      <c r="K51" s="3">
+      <c r="K51" s="1">
         <f>MIN(F51,F56,F61,F66)</f>
         <v>-148</v>
       </c>
-      <c r="L51" s="3">
+      <c r="L51" s="1">
         <f>MAX(F51,F56,F61,F66)</f>
         <v>785</v>
       </c>
-      <c r="M51" s="8">
+      <c r="M51" s="6">
         <f>AVERAGE(F51,F56,F61,F66)</f>
         <v>333.75</v>
       </c>
     </row>
     <row r="52" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
+      <c r="B52" s="1"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E52">
-        <v>15</v>
-      </c>
-      <c r="F52">
+      <c r="E52" s="8">
+        <v>15</v>
+      </c>
+      <c r="F52" s="8">
         <v>-14959</v>
       </c>
-      <c r="H52" s="14">
+      <c r="G52" s="9"/>
+      <c r="H52" s="19">
         <f>MIN(E52,E57,E62,E67)</f>
         <v>15</v>
       </c>
-      <c r="I52" s="15">
+      <c r="I52" s="11">
         <f>MAX(E52,E57,E62,E67)</f>
         <v>15</v>
       </c>
-      <c r="J52" s="10">
+      <c r="J52" s="8">
         <f>AVERAGE(E52,E57,E62,E67)</f>
         <v>15</v>
       </c>
-      <c r="K52" s="10">
+      <c r="K52" s="8">
         <f>MIN(F52,F57,F62,F67)</f>
         <v>-14959</v>
       </c>
-      <c r="L52" s="10">
+      <c r="L52" s="8">
         <f>MAX(F52,F57,F62,F67)</f>
         <v>10640</v>
       </c>
-      <c r="M52" s="11">
+      <c r="M52" s="9">
         <f>AVERAGE(F52,F57,F62,F67)</f>
         <v>-1100.5</v>
       </c>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C53" t="s">
+      <c r="B53" s="1"/>
+      <c r="C53" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="3">
         <v>2</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="3">
         <v>2345749</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="4">
         <f>AVERAGE(F53:F57)</f>
         <v>470651.6</v>
       </c>
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D54" t="s">
+      <c r="B54" s="1"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="1">
         <v>13</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="1">
         <v>1384</v>
       </c>
+      <c r="G54" s="6"/>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D55" t="s">
+      <c r="B55" s="1"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="1">
         <v>12</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="1">
         <v>9958</v>
       </c>
+      <c r="G55" s="6"/>
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D56" t="s">
+      <c r="B56" s="1"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="1">
         <v>14</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="1">
         <v>726</v>
       </c>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D57" t="s">
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="1"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E57">
-        <v>15</v>
-      </c>
-      <c r="F57">
+      <c r="E57" s="8">
+        <v>15</v>
+      </c>
+      <c r="F57" s="8">
         <v>-4559</v>
       </c>
+      <c r="G57" s="9"/>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C58" t="s">
+      <c r="B58" s="1"/>
+      <c r="C58" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="3">
         <v>4</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="3">
         <v>2134</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="4">
         <f>AVERAGE(F58:F62)</f>
         <v>93111</v>
       </c>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D59" t="s">
+      <c r="B59" s="1"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="1">
         <v>13</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="1">
         <v>-60</v>
       </c>
+      <c r="G59" s="6"/>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D60" t="s">
+      <c r="B60" s="1"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="1">
         <v>2</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="1">
         <v>459033</v>
       </c>
+      <c r="G60" s="6"/>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D61" t="s">
+      <c r="B61" s="1"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="1">
         <v>5</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="1">
         <v>-28</v>
       </c>
-    </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D62" t="s">
+      <c r="G61" s="6"/>
+    </row>
+    <row r="62" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="1"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E62">
-        <v>15</v>
-      </c>
-      <c r="F62">
+      <c r="E62" s="8">
+        <v>15</v>
+      </c>
+      <c r="F62" s="8">
         <v>4476</v>
       </c>
+      <c r="G62" s="9"/>
     </row>
     <row r="63" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C63" t="s">
+      <c r="B63" s="1"/>
+      <c r="C63" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="3">
         <v>4</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="3">
         <v>507</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="4">
         <f>AVERAGE(F63:F67)</f>
         <v>2747.2</v>
       </c>
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="D64" t="s">
+      <c r="B64" s="1"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E64">
-        <v>15</v>
-      </c>
-      <c r="F64">
+      <c r="E64" s="1">
+        <v>15</v>
+      </c>
+      <c r="F64" s="1">
         <v>962</v>
       </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D65" t="s">
+      <c r="G64" s="6"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B65" s="1"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="1">
         <v>5</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="1">
         <v>842</v>
       </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D66" t="s">
+      <c r="G65" s="6"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B66" s="1"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E66">
-        <v>15</v>
-      </c>
-      <c r="F66">
+      <c r="E66" s="1">
+        <v>15</v>
+      </c>
+      <c r="F66" s="1">
         <v>785</v>
       </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D67" t="s">
+      <c r="G66" s="6"/>
+    </row>
+    <row r="67" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="1"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E67">
-        <v>15</v>
-      </c>
-      <c r="F67">
+      <c r="E67" s="8">
+        <v>15</v>
+      </c>
+      <c r="F67" s="8">
         <v>10640</v>
       </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B69" s="2" t="s">
+      <c r="G67" s="9"/>
+    </row>
+    <row r="68" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B69" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="3">
         <v>4</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="3">
         <v>313</v>
       </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D70" t="s">
+      <c r="G69" s="4">
+        <f>AVERAGE(F69:F73)</f>
+        <v>2698</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B70" s="1"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E70">
-        <v>15</v>
-      </c>
-      <c r="F70">
+      <c r="E70" s="1">
+        <v>15</v>
+      </c>
+      <c r="F70" s="1">
         <v>966</v>
       </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D71" t="s">
+      <c r="G70" s="6"/>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B71" s="1"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="1">
         <v>9</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="1">
         <v>721</v>
       </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D72" t="s">
+      <c r="G71" s="6"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B72" s="1"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E72">
-        <v>15</v>
-      </c>
-      <c r="F72">
+      <c r="E72" s="1">
+        <v>15</v>
+      </c>
+      <c r="F72" s="1">
         <v>800</v>
       </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D73" t="s">
+      <c r="G72" s="6"/>
+    </row>
+    <row r="73" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="1"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E73">
-        <v>15</v>
-      </c>
-      <c r="F73">
+      <c r="E73" s="8">
+        <v>15</v>
+      </c>
+      <c r="F73" s="8">
         <v>10690</v>
       </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B75" s="2" t="s">
+      <c r="G73" s="9"/>
+    </row>
+    <row r="74" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="21"/>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B75" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E75">
+      <c r="E75" s="3">
         <v>4</v>
       </c>
-      <c r="F75">
+      <c r="F75" s="3">
         <v>702</v>
       </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D76" t="s">
+      <c r="G75" s="4">
+        <f>AVERAGE(F75:F79)</f>
+        <v>2797.6</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B76" s="1"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E76">
-        <v>15</v>
-      </c>
-      <c r="F76">
+      <c r="E76" s="1">
+        <v>15</v>
+      </c>
+      <c r="F76" s="1">
         <v>957</v>
       </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D77" t="s">
+      <c r="G76" s="6"/>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B77" s="1"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E77">
+      <c r="E77" s="1">
         <v>5</v>
       </c>
-      <c r="F77">
+      <c r="F77" s="1">
         <v>968</v>
       </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D78" t="s">
+      <c r="G77" s="6"/>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B78" s="1"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E78">
-        <v>15</v>
-      </c>
-      <c r="F78">
+      <c r="E78" s="1">
+        <v>15</v>
+      </c>
+      <c r="F78" s="1">
         <v>770</v>
       </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D79" t="s">
+      <c r="G78" s="6"/>
+    </row>
+    <row r="79" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="1"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E79">
-        <v>15</v>
-      </c>
-      <c r="F79">
+      <c r="E79" s="8">
+        <v>15</v>
+      </c>
+      <c r="F79" s="8">
         <v>10591</v>
       </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B81" s="2" t="s">
+      <c r="G79" s="9"/>
+    </row>
+    <row r="80" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="21"/>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B81" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="3">
         <v>4</v>
       </c>
-      <c r="F81">
+      <c r="F81" s="3">
         <v>1188</v>
       </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D82" t="s">
+      <c r="G81" s="4">
+        <f>AVERAGE(F81:F85)</f>
+        <v>2923.4</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B82" s="1"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E82">
-        <v>15</v>
-      </c>
-      <c r="F82">
+      <c r="E82" s="1">
+        <v>15</v>
+      </c>
+      <c r="F82" s="1">
         <v>946</v>
       </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D83" t="s">
+      <c r="G82" s="6"/>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B83" s="1"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="1">
         <v>5</v>
       </c>
-      <c r="F83">
+      <c r="F83" s="1">
         <v>1283</v>
       </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D84" t="s">
+      <c r="G83" s="6"/>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B84" s="1"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E84">
-        <v>15</v>
-      </c>
-      <c r="F84">
+      <c r="E84" s="1">
+        <v>15</v>
+      </c>
+      <c r="F84" s="1">
         <v>733</v>
       </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D85" t="s">
+      <c r="G84" s="6"/>
+    </row>
+    <row r="85" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="1"/>
+      <c r="C85" s="16"/>
+      <c r="D85" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E85">
-        <v>15</v>
-      </c>
-      <c r="F85">
+      <c r="E85" s="8">
+        <v>15</v>
+      </c>
+      <c r="F85" s="8">
         <v>10467</v>
+      </c>
+      <c r="G85" s="9"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B86" s="1"/>
+      <c r="C86" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" s="3">
+        <v>3</v>
+      </c>
+      <c r="F86" s="3">
+        <v>12218224</v>
+      </c>
+      <c r="G86" s="4">
+        <f>AVERAGE(F86:F90)</f>
+        <v>2451338.6</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B87" s="1"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" s="1">
+        <v>15</v>
+      </c>
+      <c r="F87" s="1">
+        <v>2703</v>
+      </c>
+      <c r="G87" s="6"/>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B88" s="1"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88" s="1">
+        <v>15</v>
+      </c>
+      <c r="F88" s="1">
+        <v>47000</v>
+      </c>
+      <c r="G88" s="6"/>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B89" s="1"/>
+      <c r="C89" s="16"/>
+      <c r="D89" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E89" s="1">
+        <v>15</v>
+      </c>
+      <c r="F89" s="1">
+        <v>2790</v>
+      </c>
+      <c r="G89" s="6"/>
+    </row>
+    <row r="90" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="1"/>
+      <c r="C90" s="16"/>
+      <c r="D90" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E90" s="8">
+        <v>15</v>
+      </c>
+      <c r="F90" s="8">
+        <v>-14024</v>
+      </c>
+      <c r="G90" s="9"/>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B91" s="1"/>
+      <c r="C91" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="3">
+        <v>2</v>
+      </c>
+      <c r="F91" s="3">
+        <v>7818900</v>
+      </c>
+      <c r="G91" s="4">
+        <f>AVERAGE(F91:F95)</f>
+        <v>1571333.4</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B92" s="1"/>
+      <c r="C92" s="16"/>
+      <c r="D92" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E92" s="1">
+        <v>13</v>
+      </c>
+      <c r="F92" s="1">
+        <v>5662</v>
+      </c>
+      <c r="G92" s="6"/>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B93" s="1"/>
+      <c r="C93" s="16"/>
+      <c r="D93" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E93" s="1">
+        <v>12</v>
+      </c>
+      <c r="F93" s="1">
+        <v>32876</v>
+      </c>
+      <c r="G93" s="6"/>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B94" s="1"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" s="1">
+        <v>14</v>
+      </c>
+      <c r="F94" s="1">
+        <v>3391</v>
+      </c>
+      <c r="G94" s="6"/>
+    </row>
+    <row r="95" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="1"/>
+      <c r="C95" s="16"/>
+      <c r="D95" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E95" s="8">
+        <v>15</v>
+      </c>
+      <c r="F95" s="8">
+        <v>-4162</v>
+      </c>
+      <c r="G95" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="26">
+        <v>0.66849999999999998</v>
+      </c>
+      <c r="E3" s="27">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="35"/>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.64044999999999996</v>
+      </c>
+      <c r="E4" s="6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="35"/>
+      <c r="C5" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="22">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="E5" s="29">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="35"/>
+      <c r="C6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.60109999999999997</v>
+      </c>
+      <c r="E6" s="9">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.64044999999999996</v>
+      </c>
+      <c r="E8" s="4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="35"/>
+      <c r="C9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.62921000000000005</v>
+      </c>
+      <c r="E9" s="6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="35"/>
+      <c r="C10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.61797999999999997</v>
+      </c>
+      <c r="E10" s="9">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.62360000000000004</v>
+      </c>
+      <c r="E12" s="4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="35"/>
+      <c r="C13" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="23">
+        <v>0.54493999999999998</v>
+      </c>
+      <c r="E13" s="31">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="35"/>
+      <c r="C14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.62360000000000004</v>
+      </c>
+      <c r="E14" s="9">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="15"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="33">
+        <v>0.58989000000000003</v>
+      </c>
+      <c r="E16" s="34">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="16"/>
+      <c r="C17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.61797999999999997</v>
+      </c>
+      <c r="E17" s="6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="16"/>
+      <c r="C18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.60670000000000002</v>
+      </c>
+      <c r="E18" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="16"/>
+      <c r="C19" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="22">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="E19" s="29">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="16"/>
+      <c r="C20" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="23">
+        <v>0.55059999999999998</v>
+      </c>
+      <c r="E20" s="31">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16"/>
+      <c r="C21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0.62360000000000004</v>
+      </c>
+      <c r="E21" s="9">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First implementation and analysis of n-gram language model.
Added normalized polar features and improved performance.
Still many TODOs and performance goals to be reached for part 4.
</commit_message>
<xml_diff>
--- a/performance_benchmarking.xlsx
+++ b/performance_benchmarking.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Selectors" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="46">
   <si>
     <t>CV</t>
   </si>
@@ -139,6 +139,33 @@
   </si>
   <si>
     <t>Constant 7</t>
+  </si>
+  <si>
+    <t>Polar_norm</t>
+  </si>
+  <si>
+    <t>Polar_norm_ext</t>
+  </si>
+  <si>
+    <t>Part 4</t>
+  </si>
+  <si>
+    <t>Basis is best solution Polar_norm_ext with DIC</t>
+  </si>
+  <si>
+    <t>Experiments and values</t>
+  </si>
+  <si>
+    <t>Normalization with exponentiation and lm_scale</t>
+  </si>
+  <si>
+    <t>LM_Scale</t>
+  </si>
+  <si>
+    <t>No influence, testing with values from 300 to 0.001</t>
+  </si>
+  <si>
+    <t>WER always stayed at 0,4551 with 97 correct words</t>
   </si>
 </sst>
 </file>
@@ -162,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +226,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -423,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -460,6 +499,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -737,14 +781,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M95"/>
+  <dimension ref="B1:M105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86:F90"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
     <col min="6" max="7" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2532,6 +2577,156 @@
       </c>
       <c r="G95" s="9"/>
     </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B96" s="1"/>
+      <c r="C96" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" s="3">
+        <v>2</v>
+      </c>
+      <c r="F96" s="3">
+        <v>19202</v>
+      </c>
+      <c r="G96" s="4">
+        <f>AVERAGE(F96:F100)</f>
+        <v>9179.4</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B97" s="1"/>
+      <c r="C97" s="16"/>
+      <c r="D97" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E97" s="1">
+        <v>14</v>
+      </c>
+      <c r="F97" s="1">
+        <v>6332</v>
+      </c>
+      <c r="G97" s="6"/>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B98" s="1"/>
+      <c r="C98" s="16"/>
+      <c r="D98" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E98" s="1">
+        <v>5</v>
+      </c>
+      <c r="F98" s="1">
+        <v>14481</v>
+      </c>
+      <c r="G98" s="6"/>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B99" s="1"/>
+      <c r="C99" s="16"/>
+      <c r="D99" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E99" s="1">
+        <v>15</v>
+      </c>
+      <c r="F99" s="1">
+        <v>1936</v>
+      </c>
+      <c r="G99" s="6"/>
+    </row>
+    <row r="100" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="1"/>
+      <c r="C100" s="16"/>
+      <c r="D100" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E100" s="8">
+        <v>14</v>
+      </c>
+      <c r="F100" s="8">
+        <v>3946</v>
+      </c>
+      <c r="G100" s="9"/>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B101" s="1"/>
+      <c r="C101" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" s="3">
+        <v>2</v>
+      </c>
+      <c r="F101" s="3">
+        <v>20005</v>
+      </c>
+      <c r="G101" s="4">
+        <f>AVERAGE(F101:F105)</f>
+        <v>11573.2</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B102" s="1"/>
+      <c r="C102" s="16"/>
+      <c r="D102" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E102" s="1">
+        <v>15</v>
+      </c>
+      <c r="F102" s="1">
+        <v>6561</v>
+      </c>
+      <c r="G102" s="6"/>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B103" s="1"/>
+      <c r="C103" s="16"/>
+      <c r="D103" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E103" s="1">
+        <v>5</v>
+      </c>
+      <c r="F103" s="1">
+        <v>15588</v>
+      </c>
+      <c r="G103" s="6"/>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B104" s="1"/>
+      <c r="C104" s="16"/>
+      <c r="D104" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E104" s="1">
+        <v>15</v>
+      </c>
+      <c r="F104" s="1">
+        <v>2176</v>
+      </c>
+      <c r="G104" s="6"/>
+    </row>
+    <row r="105" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="1"/>
+      <c r="C105" s="16"/>
+      <c r="D105" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E105" s="8">
+        <v>15</v>
+      </c>
+      <c r="F105" s="8">
+        <v>13536</v>
+      </c>
+      <c r="G105" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2539,19 +2734,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E21"/>
+  <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>29</v>
       </c>
@@ -2564,8 +2760,14 @@
       <c r="E2" s="24" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H2" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
@@ -2579,7 +2781,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="35"/>
       <c r="C4" s="5" t="s">
         <v>7</v>
@@ -2590,8 +2792,11 @@
       <c r="E4" s="6">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="35"/>
       <c r="C5" s="28" t="s">
         <v>23</v>
@@ -2602,8 +2807,11 @@
       <c r="E5" s="29">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="35"/>
       <c r="C6" s="7" t="s">
         <v>0</v>
@@ -2614,14 +2822,26 @@
       <c r="E6" s="9">
         <v>71</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6">
+        <v>200</v>
+      </c>
+      <c r="J6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="15"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="35" t="s">
         <v>6</v>
       </c>
@@ -2635,7 +2855,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="35"/>
       <c r="C9" s="5" t="s">
         <v>23</v>
@@ -2647,7 +2867,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="35"/>
       <c r="C10" s="7" t="s">
         <v>0</v>
@@ -2659,13 +2879,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="35" t="s">
         <v>4</v>
       </c>
@@ -2679,7 +2899,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="35"/>
       <c r="C13" s="30" t="s">
         <v>23</v>
@@ -2691,7 +2911,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="35"/>
       <c r="C14" s="7" t="s">
         <v>0</v>
@@ -2703,13 +2923,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="35" t="s">
         <v>5</v>
       </c>
@@ -2783,6 +3003,35 @@
         <v>67</v>
       </c>
     </row>
+    <row r="22" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="36">
+        <v>0.5393</v>
+      </c>
+      <c r="E23" s="37">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="38">
+        <v>0.4551</v>
+      </c>
+      <c r="E24" s="39">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>